<commit_message>
Version 3 - Alianzas
</commit_message>
<xml_diff>
--- a/llm_log.xlsx
+++ b/llm_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:43</t>
+          <t>2025-04-06 15:30:07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -470,7 +470,7 @@
         <is>
           <t>Extraiga los siguientes datos del texto: origen, destino, fecha, duración del viaje, tipo de viaje, acompañantes, presupuesto y expectativas.
 Texto:
-Desde dónde viaja: Pasto; Hacia dónde se dirige: costa rica; Cuándo viajar: noviembre; Duración del viaje: entre 5 y 7 días; Tipo de viaje: turismo ecológico; Con quién viaja: con un amigo; Presupuesto: entre 8 y 10 millones; Expectativas adicionales: quiero hacer avistamiento de aves
+Desde dónde viaja: pereira; Hacia dónde se dirige: roma, italia; Cuándo viajar: verano europa; Duración del viaje: 4 o 5 días; Tipo de viaje: cultural y gastronomico; Con quién viaja: solo; Presupuesto: 5 millones; Expectativas adicionales: quiero comer la mejor pasta
 Responda en formato JSON corto.</t>
         </is>
       </c>
@@ -478,14 +478,14 @@
         <is>
           <t>```json
 {
-  "origen": "Pasto",
-  "destino": "Costa Rica",
-  "fecha": "Noviembre",
-  "duracion": "5-7 días",
-  "tipo_viaje": "Turismo ecológico",
-  "acompanantes": "Un amigo",
-  "presupuesto": "8-10 millones",
-  "expectativas": "Avistamiento de aves"
+  "origen": "pereira",
+  "destino": "roma, italia",
+  "fecha": "verano europa",
+  "duracion": "4 o 5 días",
+  "tipo_viaje": "cultural y gastronomico",
+  "acompanantes": "solo",
+  "presupuesto": "5 millones",
+  "expectativas": "comer la mejor pasta"
 }
 ```</t>
         </is>
@@ -494,7 +494,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:43</t>
+          <t>2025-04-06 15:30:08</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -504,30 +504,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dado este requerimiento de viaje: ```json
-{
-  "origen": "Pasto",
-  "destino": "Costa Rica",
-  "fecha": "Noviembre",
-  "duracion": "5-7 días",
-  "tipo_viaje": "Turismo ecológico",
-  "acompanantes": "Un amigo",
-  "presupuesto": "8-10 millones",
-  "expectativas": "Avistamiento de aves"
-}
-```, genere una sola consulta de búsqueda en español (máximo una línea) para buscar los requisitos migratorios en internet.</t>
+          <t>Dado este requerimiento de viaje: {"origen": "pereira", "destino": "roma, italia"}, genere una sola consulta de búsqueda en español (máximo una línea) para buscar los requisitos migratorios en internet.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Requisitos migratorios Costa Rica desde Colombia para turismo ecológico en noviembre.</t>
+          <t>Requisitos migratorios para viajar de Pereira a Roma, Italia.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:43</t>
+          <t>2025-04-06 15:30:09</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -538,20 +527,20 @@
       <c r="C4" t="inlineStr">
         <is>
           <t>Con base en este contexto migratorio generado por el sistema:
-Requisitos migratorios Costa Rica desde Colombia para turismo ecológico en noviembre.
+Requisitos migratorios para viajar de Pereira a Roma, Italia.
 Escriba una consulta de búsqueda breve y específica en español para internet. La consulta debe buscar requisitos migratorios oficiales para ciudadanos colombianos hacia el país destino. No escriba explicaciones, solo la consulta en una línea.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Requisitos migratorios Costa Rica colombianos turismo</t>
+          <t>Requisitos migratorios Italia colombianos</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:45</t>
+          <t>2025-04-06 15:30:10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -561,23 +550,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Requisitos migratorios Costa Rica colombianos turismo</t>
+          <t>Requisitos migratorios Italia colombianos</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Requisitos Visa De Turismo Para Único Ingreso a Costa Rica: https://www.embajadadecostarica.org/wp-content/uploads/2024/12/Requisitos-visa-de-turismo-pagina-web-DC2024.pdf
-Embajada y Consulado General de Costa Rica en Colombia: https://www.embajadadecostarica.org/visas/
-Solicitar la Visa a Costa Rica de Turismo para colombianos: https://colombiacr.com.co/visaacr
-¿Qué piden a los colombianos para entrar a Costa Rica? Lista de ...: https://www.wradio.com.co/2024/05/10/que-piden-a-los-colombianos-para-entrar-a-costa-rica-lista-de-documentos-vacunas-y-mas/
-Requisitos de ingreso - Visit Costa Rica - Pautas: https://es.visitcostarica.com/planning-your-trip/entry-requirements</t>
+          <t>7 requisitos para viajar a Italia desde Colombia este 2025: https://colombianabroad.com/requisitos-entrada-italia-colombia/
+Requisitos para viajar a Italia 2025 como turista (visto): https://www.conociendoitalia.com/requisitos-para-viajar-a-italia/
+Cancillería emite recomendaciones para colombianos que viajan a Europa: https://www.cancilleria.gov.co/newsroom/news/cancilleria-emite-recomendaciones-colombianos-viajan-europa
+Esto se necesita para ir a Italia desde Colombia: Lista completa de ...: https://www.wradio.com.co/2024/04/08/esto-se-necesita-para-ir-a-italia-desde-colombia-lista-completa-de-requisitos/
+Indicaciones ingreso/salida de Colombia e ingreso a Italia: https://ambbogota.esteri.it/es/news/dall_ambasciata/2023/09/indicaciones-ingreso-salida-de-colombia-e-ingreso-a-italia/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:46</t>
+          <t>2025-04-06 15:30:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -588,35 +577,38 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>Con base en esta información y los resultados web, indique los requisitos migratorios para el viaje:
-Requisitos migratorios Costa Rica desde Colombia para turismo ecológico en noviembre.
+Requisitos migratorios para viajar de Pereira a Roma, Italia.
 Resultados de internet:
- Requisitos Visa De Turismo Para Único Ingreso a Costa Rica: https://www.embajadadecostarica.org/wp-content/uploads/2024/12/Requisitos-visa-de-turismo-pagina-web-DC2024.pdf
-Embajada y Consulado General de Costa Rica en Colombia: https://www.embajadadecostarica.org/visas/
-Solicitar la Visa a Costa Rica de Turismo para colombianos: https://colombiacr.com.co/visaacr
-¿Qué piden a los colombianos para entrar a Costa Rica? Lista de ...: https://www.wradio.com.co/2024/05/10/que-piden-a-los-colombianos-para-entrar-a-costa-rica-lista-de-documentos-vacunas-y-mas/
-Requisitos de ingreso - Visit Costa Rica - Pautas: https://es.visitcostarica.com/planning-your-trip/entry-requirements
+7 requisitos para viajar a Italia desde Colombia este 2025: https://colombianabroad.com/requisitos-entrada-italia-colombia/
+Requisitos para viajar a Italia 2025 como turista (visto): https://www.conociendoitalia.com/requisitos-para-viajar-a-italia/
+Cancillería emite recomendaciones para colombianos que viajan a Europa: https://www.cancilleria.gov.co/newsroom/news/cancilleria-emite-recomendaciones-colombianos-viajan-europa
+Esto se necesita para ir a Italia desde Colombia: Lista completa de ...: https://www.wradio.com.co/2024/04/08/esto-se-necesita-para-ir-a-italia-desde-colombia-lista-completa-de-requisitos/
+Indicaciones ingreso/salida de Colombia e ingreso a Italia: https://ambbogota.esteri.it/es/news/dall_ambasciata/2023/09/indicaciones-ingreso-salida-de-colombia-e-ingreso-a-italia/
 Sea claro y conciso. Liste si se requiere visa, vacunas u otros documentos.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Con base en la información proporcionada y los resultados web, los requisitos migratorios para colombianos que viajan a Costa Rica para turismo ecológico en noviembre son:
-*   **Visa:** Dependiendo de tu nacionalidad, es posible que necesites una visa. Consulta los enlaces proporcionados, especialmente el de la Embajada de Costa Rica en Colombia, para determinar si necesitas visa.
-*   **Pasaporte:** Pasaporte vigente con al menos seis meses de validez al momento del ingreso.
-*   **Tiquete de salida:** Billete de avión de salida de Costa Rica (ida y vuelta).
-*   **Prueba de solvencia económica:** Demostrar que se cuenta con los recursos económicos suficientes para cubrir los gastos durante la estadía.
-*   **Vacunas:** No se exigen vacunas obligatorias para ingresar a Costa Rica desde Colombia.
-*   **Otros documentos:** Es recomendable llevar una copia de la reserva del hotel o lugar de hospedaje, así como un itinerario del viaje.
-**Importante:**
-*   Verifica la información más actualizada en los sitios web oficiales de la Embajada de Costa Rica en Colombia y Visit Costa Rica, ya que los requisitos pueden cambiar.
-*   Asegúrate de cumplir con todos los requisitos para evitar problemas al ingresar al país.</t>
+          <t>Para viajar de Pereira a Roma, Italia, los requisitos migratorios generales (basados en los resultados de búsqueda y asumiendo que eres ciudadano colombiano viajando como turista en 2025) son:
+*   **Visa:** No se requiere visa para estancias turísticas cortas (hasta 90 días) dentro de un período de 180 días.
+*   **Pasaporte:** Pasaporte válido con una vigencia de al menos 3 meses después de la fecha prevista de salida de Italia/Espacio Schengen.
+*   **Tiquete de Regreso:** Billete de avión de ida y vuelta que demuestre la intención de regresar a Colombia.
+*   **Justificación del Viaje:** Documentación que justifique el propósito del viaje (ej: reservas de hotel, itinerario turístico).
+*   **Solvencia Económica:** Demostrar que se cuenta con los recursos económicos suficientes para cubrir los gastos durante la estancia. Esto puede ser en efectivo, tarjetas de crédito, cheques de viajero, etc. Se recomienda verificar el monto mínimo requerido actualizado para 2025.
+*   **Seguro de Viaje:** Es obligatorio contar con un seguro de viaje con cobertura médica internacional que cubra gastos de hospitalización y repatriación, con una cobertura mínima de 30.000 euros.
+*   **Vacunas:** No hay vacunas obligatorias para ingresar a Italia desde Colombia, pero se recomienda consultar con un médico sobre las vacunas recomendadas para viajes internacionales.
+*   **Formulario de localización de pasajeros (PLF):** Es posible que se requiera completar un formulario de localización de pasajeros (PLF) antes de viajar. Esto dependerá de las regulaciones sanitarias vigentes en el momento del viaje.
+**Recomendaciones Adicionales:**
+*   **Consulta las fuentes oficiales:** Verifica la información directamente en las páginas web de la Embajada de Italia en Colombia y la Cancillería de Colombia para obtener la información más actualizada y precisa.
+*   **Considera posibles cambios:** Los requisitos pueden cambiar, especialmente en lo relacionado con la pandemia. Mantente informado cerca de la fecha de tu viaje.
+**Nota:** Esta información es una guía general. Es fundamental verificar los requisitos específicos y actualizados en las fuentes oficiales antes de viajar.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:48</t>
+          <t>2025-04-06 15:30:15</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -627,34 +619,23 @@
       <c r="C7" t="inlineStr">
         <is>
           <t>Describa brevemente el clima, las temporadas turísticas (alta o baja) y eventos relevantes en el destino según esta información:
-```json
-{
-  "origen": "Pasto",
-  "destino": "Costa Rica",
-  "fecha": "Noviembre",
-  "duracion": "5-7 días",
-  "tipo_viaje": "Turismo ecológico",
-  "acompanantes": "Un amigo",
-  "presupuesto": "8-10 millones",
-  "expectativas": "Avistamiento de aves"
-}
-```
+roma, italia, verano europa
 Use viñetas si es posible. Sea claro y evite detalles innecesarios.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Basado en la información proporcionada para un viaje a Costa Rica en Noviembre:
-*   **Clima:** Noviembre marca el final de la temporada de lluvias en la mayor parte de Costa Rica, especialmente en la costa del Pacífico. Se pueden esperar lluvias intermitentes, pero también días soleados. La costa del Caribe tiende a ser más lluviosa en esta época.
-*   **Temporada Turística:** Noviembre se considera temporada baja/media. Los precios suelen ser más bajos que en la temporada alta (Diciembre-Abril) y hay menos multitudes.
-*   **Eventos Relevantes:** Aunque no hay eventos nacionales específicos mencionados, Noviembre es un buen mes para el avistamiento de aves migratorias, lo que se alinea con las expectativas del viaje.</t>
+          <t>Aquí tienes una descripción concisa del clima, temporadas turísticas y eventos en Roma, Italia, durante el verano europeo:
+*   **Clima:** Caluroso y seco. Temperaturas elevadas, especialmente en julio y agosto.
+*   **Temporada Turística:** Alta. El verano es la temporada más popular para visitar Roma, por lo que hay mucha gente y precios más altos.
+*   **Eventos Relevantes:** Festivales al aire libre, conciertos, eventos culturales y celebraciones religiosas.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:48</t>
+          <t>2025-04-06 15:30:15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -665,23 +646,23 @@
       <c r="C8" t="inlineStr">
         <is>
           <t>Según este contexto turístico:
-Basado en la información proporcionada para un viaje a Costa Rica en Noviembre:
-*   **Clima:** Noviembre marca el final de la temporada de lluvias en la mayor parte de Costa Rica, especialmente en la costa del Pacífico. Se pueden esperar lluvias intermitentes, pero también días soleados. La costa del Caribe tiende a ser más lluviosa en esta época.
-*   **Temporada Turística:** Noviembre se considera temporada baja/media. Los precios suelen ser más bajos que en la temporada alta (Diciembre-Abril) y hay menos multitudes.
-*   **Eventos Relevantes:** Aunque no hay eventos nacionales específicos mencionados, Noviembre es un buen mes para el avistamiento de aves migratorias, lo que se alinea con las expectativas del viaje.
+Aquí tienes una descripción concisa del clima, temporadas turísticas y eventos en Roma, Italia, durante el verano europeo:
+*   **Clima:** Caluroso y seco. Temperaturas elevadas, especialmente en julio y agosto.
+*   **Temporada Turística:** Alta. El verano es la temporada más popular para visitar Roma, por lo que hay mucha gente y precios más altos.
+*   **Eventos Relevantes:** Festivales al aire libre, conciertos, eventos culturales y celebraciones religiosas.
 Genere una consulta de búsqueda concreta y corta en español para internet. Debe enfocarse en eventos turísticos, clima o temporadas en el destino en las fechas del viaje. No incluya explicaciones, solo la consulta.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Costa Rica Noviembre clima eventos turísticos</t>
+          <t>Roma eventos verano precios</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:49</t>
+          <t>2025-04-06 15:30:17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -691,23 +672,23 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Costa Rica Noviembre clima eventos turísticos</t>
+          <t>Roma eventos verano precios</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Viajar a Costa Rica en Noviembre: el tiempo y recomendaciones: https://guiadeviajeacostarica.com/noviembre-el-tiempo/
-¿Por Qué Viajar a Costa Rica en Noviembre?: https://viajesacostarica.es/costa-rica-en-noviembre/
-Costa Rica Weather In November - Everything You Must Know: https://www.findmycostarica.com/blog/costa-rica-weather-in-november/
-Costa Rica en noviembre: Ideas de viaje, clima y más: http://grainofsound.org/es/costa-rica-en-noviembre-ideas-de-viaje-clima-y-más/
-Temperatura Promedio Y Condiciones Climáticas En Costa Rica En Noviembre: https://roambliss.com/es/temperatura-en-costa-rica-en-noviembre/</t>
+          <t>Eventos, calendario y entradas en Roma, Italia | Eventbrite: https://www.eventbrite.es/d/italy--roma/events/
+Eventos en Roma, próximos eventos, todos los eventos ... - 10times: https://10times.com/es/rome-it
+Verano en Roma: Eventos, Festivales y Vida Nocturna: https://www.romeprivateguides.com/es/blog/sobre-roma/to-do-summer-rome.html
+Eventos en Roma, música, cine y espectáculos - Guía en Roma: https://www.enroma.com/eventos-roma/
+10 cosas que hacer en Roma en verano - Hellotickets: https://www.hellotickets.es/italia/roma/roma-en-verano/sc-124-2092</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:51</t>
+          <t>2025-04-06 15:30:18</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -718,39 +699,37 @@
       <c r="C10" t="inlineStr">
         <is>
           <t>Utilice la siguiente información y resultados de búsqueda para resumir el clima, eventos y temporada turística del destino:
-Basado en la información proporcionada para un viaje a Costa Rica en Noviembre:
-*   **Clima:** Noviembre marca el final de la temporada de lluvias en la mayor parte de Costa Rica, especialmente en la costa del Pacífico. Se pueden esperar lluvias intermitentes, pero también días soleados. La costa del Caribe tiende a ser más lluviosa en esta época.
-*   **Temporada Turística:** Noviembre se considera temporada baja/media. Los precios suelen ser más bajos que en la temporada alta (Diciembre-Abril) y hay menos multitudes.
-*   **Eventos Relevantes:** Aunque no hay eventos nacionales específicos mencionados, Noviembre es un buen mes para el avistamiento de aves migratorias, lo que se alinea con las expectativas del viaje.
+Aquí tienes una descripción concisa del clima, temporadas turísticas y eventos en Roma, Italia, durante el verano europeo:
+*   **Clima:** Caluroso y seco. Temperaturas elevadas, especialmente en julio y agosto.
+*   **Temporada Turística:** Alta. El verano es la temporada más popular para visitar Roma, por lo que hay mucha gente y precios más altos.
+*   **Eventos Relevantes:** Festivales al aire libre, conciertos, eventos culturales y celebraciones religiosas.
 Resultados de internet:
-Viajar a Costa Rica en Noviembre: el tiempo y recomendaciones: https://guiadeviajeacostarica.com/noviembre-el-tiempo/
-¿Por Qué Viajar a Costa Rica en Noviembre?: https://viajesacostarica.es/costa-rica-en-noviembre/
-Costa Rica Weather In November - Everything You Must Know: https://www.findmycostarica.com/blog/costa-rica-weather-in-november/
-Costa Rica en noviembre: Ideas de viaje, clima y más: http://grainofsound.org/es/costa-rica-en-noviembre-ideas-de-viaje-clima-y-más/
-Temperatura Promedio Y Condiciones Climáticas En Costa Rica En Noviembre: https://roambliss.com/es/temperatura-en-costa-rica-en-noviembre/
+Eventos, calendario y entradas en Roma, Italia | Eventbrite: https://www.eventbrite.es/d/italy--roma/events/
+Eventos en Roma, próximos eventos, todos los eventos ... - 10times: https://10times.com/es/rome-it
+Verano en Roma: Eventos, Festivales y Vida Nocturna: https://www.romeprivateguides.com/es/blog/sobre-roma/to-do-summer-rome.html
+Eventos en Roma, música, cine y espectáculos - Guía en Roma: https://www.enroma.com/eventos-roma/
+10 cosas que hacer en Roma en verano - Hellotickets: https://www.hellotickets.es/italia/roma/roma-en-verano/sc-124-2092
 Use viñetas si es posible. Sea concreto.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Aquí está un resumen del clima, eventos y temporada turística en Costa Rica en Noviembre, basado en la información proporcionada y los resultados de búsqueda:
-*   **Clima:** Noviembre representa la transición de la temporada de lluvias a la seca.
-    *   **Pacífico:** Disminuyen las lluvias, con días soleados intercalados.
-    *   **Caribe:** Generalmente más lluvioso que el Pacífico.
-    *   En general, se puede esperar lluvia, pero no constante.
-*   **Temporada Turística:** Temporada baja/media.
-    *   Menos multitudes en comparación con la temporada alta (Diciembre-Abril).
-    *   Precios más bajos en alojamiento y tours.
-*   **Eventos/Actividades:**
-    *   Avistamiento de aves migratorias (oportunidad destacada).
-    *   Aunque no se mencionan eventos nacionales específicos, el clima en transición y la menor afluencia de turistas hacen de Noviembre un buen momento para explorar el país.</t>
+          <t>Aquí está un resumen del clima, eventos y temporada turística en Roma durante el verano europeo:
+*   **Clima:** Caluroso y seco, con temperaturas elevadas, especialmente en julio y agosto.
+*   **Temporada Turística:** Alta. El verano es la temporada turística más popular, lo que significa multitudes y precios más altos.
+*   **Eventos:**
+    *   Festivales al aire libre.
+    *   Conciertos.
+    *   Eventos culturales.
+    *   Celebraciones religiosas.
+    *   Una variedad de eventos listados en plataformas como Eventbrite, 10times, Rome Private Guides, Guía en Roma y Hellotickets.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:58</t>
+          <t>2025-04-06 15:30:24</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -760,77 +739,69 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Con base en la información del viaje, estime el costo diario en COP de:
-- Transporte
-- Alojamiento
-- Comida
+          <t>Con base en la información del viaje y el número de viajeros, estime:
+- Costo total diario en COP de transporte (tiquetes incluidos), alojamiento y comida.
+- Costo diario por persona en COP para cada concepto.
 Datos:
-```json
-{
-  "origen": "Pasto",
-  "destino": "Costa Rica",
-  "fecha": "Noviembre",
-  "duracion": "5-7 días",
-  "tipo_viaje": "Turismo ecológico",
-  "acompanantes": "Un amigo",
-  "presupuesto": "8-10 millones",
-  "expectativas": "Avistamiento de aves"
-}
-```
-Presente el valor aproximado por cada concepto.</t>
+{"origen": "pereira", "destino": "roma, italia", "duracion": "4", "tipo_viaje": "cultural y gastronomico"}
+Presente valores totales y por persona.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Okay, vamos a estimar el costo diario en COP para transporte, alojamiento y comida, basándonos en la información proporcionada para un viaje de Pasto a Costa Rica, con un enfoque en turismo ecológico y avistamiento de aves.
-**Consideraciones Importantes:**
-*   **Conversión:** Asumiremos una tasa de cambio aproximada de 1 USD = 4000 COP (esta tasa puede variar).
-*   **Rango de Duración:** Tomaremos el punto medio de la duración del viaje (6 días) para calcular los costos diarios.
-*   **Presupuesto Total:** Usaremos el punto medio del presupuesto (9 millones COP) como referencia.
-*   **Tipo de Viaje:** El turismo ecológico generalmente implica opciones de alojamiento y comida más económicas que el turismo de lujo, pero puede requerir transporte especializado para acceder a áreas naturales.
-*   **Acompañante:** Dividiremos algunos costos (como alojamiento) entre dos personas.
-**Estimación de Costos Diarios (COP):**
-**1. Transporte:**
-*   **Vuelos:** El costo del vuelo Pasto - Costa Rica (ida y vuelta) es la parte más significativa.  Un vuelo de ida y vuelta puede costar entre 2.000.000 COP y 4.000.000 COP por persona, dependiendo de la aerolínea, la temporada y la anticipación con la que se compre.  Para dos personas, esto sería entre 4.000.000 COP y 8.000.000 COP.
-*   **Transporte Interno en Costa Rica:**  Dado el enfoque en turismo ecológico y avistamiento de aves, es probable que se necesite transporte para acceder a parques nacionales, reservas y otros sitios de interés. Esto podría incluir:
-    *   **Alquiler de coche:**  Puede costar entre 120.000 COP y 200.000 COP por día (dividido entre dos personas).
-    *   **Transporte público (autobuses):** Una opción más económica, pero menos flexible.  Podría costar entre 20.000 COP y 50.000 COP por persona por día.
-    *   **Taxis/Uber:**  Para distancias cortas, pero puede ser costoso para traslados largos.
-    *   **Traslados privados/Shuttles:**  Comunes para llegar a lodges ecológicos.  Pueden costar entre 50.000 COP y 100.000 COP por persona por trayecto.
-*   **Costo Diario Estimado de Transporte:**
-    *   **Vuelos:** (4.000.000 COP / 6 días) = 666.667 COP por persona.
-    *   **Transporte Interno:** Asumiremos un promedio de 100.000 COP por persona por día (combinación de alquiler de coche compartido, transporte público y traslados ocasionales).
-    *   **Total Transporte Diario:** 666.667 COP + 100.000 COP = **766.667 COP por persona**.
-**2. Alojamiento:**
-*   **Opciones:**  Costa Rica ofrece una amplia gama de alojamientos, desde hostales económicos hasta lodges de lujo.  Dado el presupuesto y el enfoque en turismo ecológico, asumiremos opciones de rango medio, como:
-    *   **Hostales/Cabañas:** 50.000 COP - 100.000 COP por persona por noche.
-    *   **Hoteles Ecológicos/B&amp;B:** 100.000 COP - 200.000 COP por persona por noche.
-*   **Costo Diario Estimado de Alojamiento:**  Asumiremos un promedio de 150.000 COP por persona por noche.
-**3. Comida:**
-*   **Opciones:**  Los costos de comida pueden variar significativamente dependiendo de dónde se coma.
-    *   **Restaurantes locales (sodas):**  Comidas económicas (20.000 COP - 40.000 COP por comida).
-    *   **Restaurantes turísticos:**  Más caros (50.000 COP - 100.000 COP por comida).
-    *   **Supermercados:**  Para comprar provisiones y reducir costos.
-*   **Costo Diario Estimado de Comida:**  Asumiremos un promedio de 100.000 COP por persona por día (combinando comidas en restaurantes locales, algunas comidas en restaurantes turísticos y compras en supermercados).
-**Resumen del Costo Diario Estimado (COP):**
-*   **Transporte:** 766.667 COP
-*   **Alojamiento:** 150.000 COP
-*   **Comida:** 100.000 COP
-*   **Total Diario Estimado:** **1.016.667 COP por persona**
-**Consideraciones Finales:**
-*   **Actividades:**  Este cálculo no incluye el costo de actividades como tours de avistamiento de aves, entradas a parques nacionales, etc.  Estos costos pueden variar significativamente.  Es importante investigar y presupuestar estas actividades por separado.
-*   **Seguro de Viaje:**  Es fundamental contar con un seguro de viaje, lo cual agregaría un costo adicional.
-*   **Flexibilidad:**  Es importante tener flexibilidad en el presupuesto, ya que pueden surgir gastos inesperados.
-*   **Negociación:**  En algunos casos, es posible negociar precios, especialmente en alojamientos y tours locales.
+          <t>Para estimar el costo del viaje, necesito hacer algunas suposiciones y usar rangos de precios promedio, ya que la información proporcionada es limitada.  Es importante recordar que estos son solo estimados y los precios reales pueden variar significativamente dependiendo de las elecciones específicas (aerolínea, hotel, restaurantes, etc.).
+**Suposiciones:**
+*   **Tiquetes:** Asumo un precio promedio para un tiquete ida y vuelta Pereira - Roma.
+*   **Alojamiento:** Asumo un hotel de gama media (3 estrellas) o un Airbnb con buena ubicación.
+*   **Comida:** Asumo un presupuesto moderado para comidas, incluyendo restaurantes locales y algunas experiencias gastronómicas.
+*   **Transporte local:** Incluyo transporte público y algunos taxis/ubers.
+*   **Número de viajeros:** Asumo que viaja **1 persona**, ya que no se especifica. Si viajan más personas, el costo por persona de alojamiento podría disminuir.
+**Estimaciones:**
+**1. Tiquetes (Ida y Vuelta Pereira - Roma):**
+*   Rango estimado: COP 4.000.000 - COP 7.000.000 (Dependiendo de la temporada, aerolínea y anticipación de la compra).
+*   Promedio estimado: COP 5.500.000
+**2. Alojamiento (por noche):**
+*   Rango estimado: COP 300.000 - COP 600.000 (Hotel 3 estrellas o Airbnb bien ubicado).
+*   Promedio estimado: COP 450.000
+**3. Comida (por día):**
+*   Rango estimado: COP 150.000 - COP 300.000 (Incluyendo desayuno, almuerzo, cena y alguna experiencia gastronómica).
+*   Promedio estimado: COP 225.000
+**4. Transporte Local (por día):**
+*   Rango estimado: COP 30.000 - COP 60.000 (Transporte público, algunos taxis/ubers).
+*   Promedio estimado: COP 45.000
+**Cálculos:**
+*   **Costo total de alojamiento (4 noches):** 4 noches * COP 450.000/noche = COP 1.800.000
+*   **Costo total de comida (4 días):** 4 días * COP 225.000/día = COP 900.000
+*   **Costo total de transporte local (4 días):** 4 días * COP 45.000/día = COP 180.000
+**Resumen:**
+| Concepto        | Costo Total (COP) | Costo Diario (COP) | Costo Diario por Persona (COP) |
+|-----------------|--------------------|---------------------|---------------------------------|
+| Tiquetes        | 5.500.000          | 1.375.000 (prorrateado)  | 1.375.000                       |
+| Alojamiento     | 1.800.000          | 450.000             | 450.000                         |
+| Comida          | 900.000            | 225.000             | 225.000                         |
+| Transporte Local | 180.000            | 45.000              | 45.000                          |
+| **TOTAL**       | **8.380.000**      | **2.095.000**       | **2.095.000**                   |
 **Conclusión:**
-Con un presupuesto de 9 millones de COP para dos personas durante 6 días, el costo diario estimado de 1.016.667 COP por persona parece razonable, aunque es importante tener en cuenta las consideraciones finales y ajustar el presupuesto según las preferencias y actividades específicas del viaje.  Es crucial investigar los precios de los vuelos y alojamientos con anticipación para obtener una estimación más precisa.</t>
+*   **Costo total estimado del viaje (4 días): COP 8.380.000**
+*   **Costo total diario estimado: COP 2.095.000**
+*   **Costo diario por persona estimado: COP 2.095.000**
+**Importante:**
+*   Estos son solo estimados.  Investigue a fondo los precios de vuelos y alojamiento para obtener una estimación más precisa.
+*   El costo de las actividades culturales (museos, tours, etc.) y otros gastos (souvenirs, etc.) no están incluidos en esta estimación.
+*   Los precios pueden variar significativamente dependiendo de la temporada alta/baja y la disponibilidad.
+*   Considere la tasa de cambio COP/EUR al momento de planificar su viaje.
+Para obtener una estimación más precisa, proporcione:
+*   Fechas específicas del viaje.
+*   Número de viajeros.
+*   Preferencias de alojamiento (hotel, Airbnb, presupuesto).
+*   Intereses específicos (actividades, restaurantes).</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-04-05 20:04:59</t>
+          <t>2025-04-06 15:30:25</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -840,62 +811,68 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Este es un resumen de contexto sobre los costos estimados del viaje:
-Okay, vamos a estimar el costo diario en COP para transporte, alojamiento y comida, basándonos en la información proporcionada para un viaje de Pasto a Costa Rica, con un enfoque en turismo ecológico y avistamiento de aves.
-**Consideraciones Importantes:**
-*   **Conversión:** Asumiremos una tasa de cambio aproximada de 1 USD = 4000 COP (esta tasa puede variar).
-*   **Rango de Duración:** Tomaremos el punto medio de la duración del viaje (6 días) para calcular los costos diarios.
-*   **Presupuesto Total:** Usaremos el punto medio del presupuesto (9 millones COP) como referencia.
-*   **Tipo de Viaje:** El turismo ecológico generalmente implica opciones de alojamiento y comida más económicas que el turismo de lujo, pero puede requerir transporte especializado para acceder a áreas naturales.
-*   **Acompañante:** Dividiremos algunos costos (como alojamiento) entre dos personas.
-**Estimación de Costos Diarios (COP):**
-**1. Transporte:**
-*   **Vuelos:** El costo del vuelo Pasto - Costa Rica (ida y vuelta) es la parte más significativa.  Un vuelo de ida y vuelta puede costar entre 2.000.000 COP y 4.000.000 COP por persona, dependiendo de la aerolínea, la temporada y la anticipación con la que se compre.  Para dos personas, esto sería entre 4.000.000 COP y 8.000.000 COP.
-*   **Transporte Interno en Costa Rica:**  Dado el enfoque en turismo ecológico y avistamiento de aves, es probable que se necesite transporte para acceder a parques nacionales, reservas y otros sitios de interés. Esto podría incluir:
-    *   **Alquiler de coche:**  Puede costar entre 120.000 COP y 200.000 COP por día (dividido entre dos personas).
-    *   **Transporte público (autobuses):** Una opción más económica, pero menos flexible.  Podría costar entre 20.000 COP y 50.000 COP por persona por día.
-    *   **Taxis/Uber:**  Para distancias cortas, pero puede ser costoso para traslados largos.
-    *   **Traslados privados/Shuttles:**  Comunes para llegar a lodges ecológicos.  Pueden costar entre 50.000 COP y 100.000 COP por persona por trayecto.
-*   **Costo Diario Estimado de Transporte:**
-    *   **Vuelos:** (4.000.000 COP / 6 días) = 666.667 COP por persona.
-    *   **Transporte Interno:** Asumiremos un promedio de 100.000 COP por persona por día (combinación de alquiler de coche compartido, transporte público y traslados ocasionales).
-    *   **Total Transporte Diario:** 666.667 COP + 100.000 COP = **766.667 COP por persona**.
-**2. Alojamiento:**
-*   **Opciones:**  Costa Rica ofrece una amplia gama de alojamientos, desde hostales económicos hasta lodges de lujo.  Dado el presupuesto y el enfoque en turismo ecológico, asumiremos opciones de rango medio, como:
-    *   **Hostales/Cabañas:** 50.000 COP - 100.000 COP por persona por noche.
-    *   **Hoteles Ecológicos/B&amp;B:** 100.000 COP - 200.000 COP por persona por noche.
-*   **Costo Diario Estimado de Alojamiento:**  Asumiremos un promedio de 150.000 COP por persona por noche.
-**3. Comida:**
-*   **Opciones:**  Los costos de comida pueden variar significativamente dependiendo de dónde se coma.
-    *   **Restaurantes locales (sodas):**  Comidas económicas (20.000 COP - 40.000 COP por comida).
-    *   **Restaurantes turísticos:**  Más caros (50.000 COP - 100.000 COP por comida).
-    *   **Supermercados:**  Para comprar provisiones y reducir costos.
-*   **Costo Diario Estimado de Comida:**  Asumiremos un promedio de 100.000 COP por persona por día (combinando comidas en restaurantes locales, algunas comidas en restaurantes turísticos y compras en supermercados).
-**Resumen del Costo Diario Estimado (COP):**
-*   **Transporte:** 766.667 COP
-*   **Alojamiento:** 150.000 COP
-*   **Comida:** 100.000 COP
-*   **Total Diario Estimado:** **1.016.667 COP por persona**
-**Consideraciones Finales:**
-*   **Actividades:**  Este cálculo no incluye el costo de actividades como tours de avistamiento de aves, entradas a parques nacionales, etc.  Estos costos pueden variar significativamente.  Es importante investigar y presupuestar estas actividades por separado.
-*   **Seguro de Viaje:**  Es fundamental contar con un seguro de viaje, lo cual agregaría un costo adicional.
-*   **Flexibilidad:**  Es importante tener flexibilidad en el presupuesto, ya que pueden surgir gastos inesperados.
-*   **Negociación:**  En algunos casos, es posible negociar precios, especialmente en alojamientos y tours locales.
+          <t>Resumen de contexto sobre costos estimados:
+Para estimar el costo del viaje, necesito hacer algunas suposiciones y usar rangos de precios promedio, ya que la información proporcionada es limitada.  Es importante recordar que estos son solo estimados y los precios reales pueden variar significativamente dependiendo de las elecciones específicas (aerolínea, hotel, restaurantes, etc.).
+**Suposiciones:**
+*   **Tiquetes:** Asumo un precio promedio para un tiquete ida y vuelta Pereira - Roma.
+*   **Alojamiento:** Asumo un hotel de gama media (3 estrellas) o un Airbnb con buena ubicación.
+*   **Comida:** Asumo un presupuesto moderado para comidas, incluyendo restaurantes locales y algunas experiencias gastronómicas.
+*   **Transporte local:** Incluyo transporte público y algunos taxis/ubers.
+*   **Número de viajeros:** Asumo que viaja **1 persona**, ya que no se especifica. Si viajan más personas, el costo por persona de alojamiento podría disminuir.
+**Estimaciones:**
+**1. Tiquetes (Ida y Vuelta Pereira - Roma):**
+*   Rango estimado: COP 4.000.000 - COP 7.000.000 (Dependiendo de la temporada, aerolínea y anticipación de la compra).
+*   Promedio estimado: COP 5.500.000
+**2. Alojamiento (por noche):**
+*   Rango estimado: COP 300.000 - COP 600.000 (Hotel 3 estrellas o Airbnb bien ubicado).
+*   Promedio estimado: COP 450.000
+**3. Comida (por día):**
+*   Rango estimado: COP 150.000 - COP 300.000 (Incluyendo desayuno, almuerzo, cena y alguna experiencia gastronómica).
+*   Promedio estimado: COP 225.000
+**4. Transporte Local (por día):**
+*   Rango estimado: COP 30.000 - COP 60.000 (Transporte público, algunos taxis/ubers).
+*   Promedio estimado: COP 45.000
+**Cálculos:**
+*   **Costo total de alojamiento (4 noches):** 4 noches * COP 450.000/noche = COP 1.800.000
+*   **Costo total de comida (4 días):** 4 días * COP 225.000/día = COP 900.000
+*   **Costo total de transporte local (4 días):** 4 días * COP 45.000/día = COP 180.000
+**Resumen:**
+| Concepto        | Costo Total (COP) | Costo Diario (COP) | Costo Diario por Persona (COP) |
+|-----------------|--------------------|---------------------|---------------------------------|
+| Tiquetes        | 5.500.000          | 1.375.000 (prorrateado)  | 1.375.000                       |
+| Alojamiento     | 1.800.000          | 450.000             | 450.000                         |
+| Comida          | 900.000            | 225.000             | 225.000                         |
+| Transporte Local | 180.000            | 45.000              | 45.000                          |
+| **TOTAL**       | **8.380.000**      | **2.095.000**       | **2.095.000**                   |
 **Conclusión:**
-Con un presupuesto de 9 millones de COP para dos personas durante 6 días, el costo diario estimado de 1.016.667 COP por persona parece razonable, aunque es importante tener en cuenta las consideraciones finales y ajustar el presupuesto según las preferencias y actividades específicas del viaje.  Es crucial investigar los precios de los vuelos y alojamientos con anticipación para obtener una estimación más precisa.
-Cree una consulta en español (una línea) para buscar en internet información sobre precios promedio en transporte, alojamiento o comida en el destino turístico. Enfóquese en el país y ciudad destino, si se conoce. No escriba justificaciones, solo la consulta.</t>
+*   **Costo total estimado del viaje (4 días): COP 8.380.000**
+*   **Costo total diario estimado: COP 2.095.000**
+*   **Costo diario por persona estimado: COP 2.095.000**
+**Importante:**
+*   Estos son solo estimados.  Investigue a fondo los precios de vuelos y alojamiento para obtener una estimación más precisa.
+*   El costo de las actividades culturales (museos, tours, etc.) y otros gastos (souvenirs, etc.) no están incluidos en esta estimación.
+*   Los precios pueden variar significativamente dependiendo de la temporada alta/baja y la disponibilidad.
+*   Considere la tasa de cambio COP/EUR al momento de planificar su viaje.
+Para obtener una estimación más precisa, proporcione:
+*   Fechas específicas del viaje.
+*   Número de viajeros.
+*   Preferencias de alojamiento (hotel, Airbnb, presupuesto).
+*   Intereses específicos (actividades, restaurantes).
+Genere una consulta en español (una línea) para buscar en internet:
+- Precio promedio de transporte local, alojamiento y comida en el destino.
+No incluya explicaciones, solo la consulta.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Precios promedio transporte alojamiento comida Costa Rica San José</t>
+          <t>costo promedio transporte alojamiento comida Roma</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-04-05 20:05:42</t>
+          <t>2025-04-06 15:31:07</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -905,23 +882,23 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Precios promedio transporte alojamiento comida Costa Rica San José</t>
+          <t>costo promedio transporte alojamiento comida Roma</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Precios en San José Marzo 2025 precios en restaurantes, alimentos y ...: https://hikersbay.com/prices/costarica/p/san-jose?lang=es
-Costo de vida y precios en San José ... - TravelTables: https://es.traveltables.com/country/costa-rica/city/san-jose/cost-of-living/
-Precios de transportes y servicios en Costa Rica 2025: https://preciosmundi.com/costa-rica/precio-transporte-servicios
-Costo de vida en San Jose, Costa Rica, Costa Rica - Expatistan: https://www.expatistan.com/es/costo-de-vida/san-jose-costa-rica
-Costo de viaje: Guía económica de Costa Rica | El Blog del Viajero: https://elblogdelviajero.com/costo-de-viaje-costa-rica-2/</t>
+          <t>Precios en Roma 2025 precios en restaurantes, alimentos y bebidas ...: https://hikersbay.com/prices/italy/rome?lang=es
+¿Cuánto dinero se necesita para visitar Roma? - HolboxPhotos: https://holboxphotos.com/roma/cuanto-dinero-se-necesita-para-visitar-roma/
+¿Cuánto dinero se gasta por día en Roma? | Felices Vacaciones: https://blog.felicesvacaciones.es/cuanto-dinero-se-gasta-por-dia-en-roma
+Precios en Roma, Transporte, Comida y bebidas, Alojamiento, Turismo: https://www.viajarroma.com/precios/
+¿Cuánto cuesta un viaje a Roma? Todos los días, 3 días y por semana ...: https://hikersbay.com/travel-cost/italy/rome?lang=es</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-04-05 20:05:42</t>
+          <t>2025-04-06 15:31:08</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -931,260 +908,546 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Con base en la información siguiente, entregue una estimación de costos diarios en COP para:
-- Transporte
-- Alojamiento
-- Alimentación
-Okay, vamos a estimar el costo diario en COP para transporte, alojamiento y comida, basándonos en la información proporcionada para un viaje de Pasto a Costa Rica, con un enfoque en turismo ecológico y avistamiento de aves.
-**Consideraciones Importantes:**
-*   **Conversión:** Asumiremos una tasa de cambio aproximada de 1 USD = 4000 COP (esta tasa puede variar).
-*   **Rango de Duración:** Tomaremos el punto medio de la duración del viaje (6 días) para calcular los costos diarios.
-*   **Presupuesto Total:** Usaremos el punto medio del presupuesto (9 millones COP) como referencia.
-*   **Tipo de Viaje:** El turismo ecológico generalmente implica opciones de alojamiento y comida más económicas que el turismo de lujo, pero puede requerir transporte especializado para acceder a áreas naturales.
-*   **Acompañante:** Dividiremos algunos costos (como alojamiento) entre dos personas.
-**Estimación de Costos Diarios (COP):**
-**1. Transporte:**
-*   **Vuelos:** El costo del vuelo Pasto - Costa Rica (ida y vuelta) es la parte más significativa.  Un vuelo de ida y vuelta puede costar entre 2.000.000 COP y 4.000.000 COP por persona, dependiendo de la aerolínea, la temporada y la anticipación con la que se compre.  Para dos personas, esto sería entre 4.000.000 COP y 8.000.000 COP.
-*   **Transporte Interno en Costa Rica:**  Dado el enfoque en turismo ecológico y avistamiento de aves, es probable que se necesite transporte para acceder a parques nacionales, reservas y otros sitios de interés. Esto podría incluir:
-    *   **Alquiler de coche:**  Puede costar entre 120.000 COP y 200.000 COP por día (dividido entre dos personas).
-    *   **Transporte público (autobuses):** Una opción más económica, pero menos flexible.  Podría costar entre 20.000 COP y 50.000 COP por persona por día.
-    *   **Taxis/Uber:**  Para distancias cortas, pero puede ser costoso para traslados largos.
-    *   **Traslados privados/Shuttles:**  Comunes para llegar a lodges ecológicos.  Pueden costar entre 50.000 COP y 100.000 COP por persona por trayecto.
-*   **Costo Diario Estimado de Transporte:**
-    *   **Vuelos:** (4.000.000 COP / 6 días) = 666.667 COP por persona.
-    *   **Transporte Interno:** Asumiremos un promedio de 100.000 COP por persona por día (combinación de alquiler de coche compartido, transporte público y traslados ocasionales).
-    *   **Total Transporte Diario:** 666.667 COP + 100.000 COP = **766.667 COP por persona**.
-**2. Alojamiento:**
-*   **Opciones:**  Costa Rica ofrece una amplia gama de alojamientos, desde hostales económicos hasta lodges de lujo.  Dado el presupuesto y el enfoque en turismo ecológico, asumiremos opciones de rango medio, como:
-    *   **Hostales/Cabañas:** 50.000 COP - 100.000 COP por persona por noche.
-    *   **Hoteles Ecológicos/B&amp;B:** 100.000 COP - 200.000 COP por persona por noche.
-*   **Costo Diario Estimado de Alojamiento:**  Asumiremos un promedio de 150.000 COP por persona por noche.
-**3. Comida:**
-*   **Opciones:**  Los costos de comida pueden variar significativamente dependiendo de dónde se coma.
-    *   **Restaurantes locales (sodas):**  Comidas económicas (20.000 COP - 40.000 COP por comida).
-    *   **Restaurantes turísticos:**  Más caros (50.000 COP - 100.000 COP por comida).
-    *   **Supermercados:**  Para comprar provisiones y reducir costos.
-*   **Costo Diario Estimado de Comida:**  Asumiremos un promedio de 100.000 COP por persona por día (combinando comidas en restaurantes locales, algunas comidas en restaurantes turísticos y compras en supermercados).
-**Resumen del Costo Diario Estimado (COP):**
-*   **Transporte:** 766.667 COP
-*   **Alojamiento:** 150.000 COP
-*   **Comida:** 100.000 COP
-*   **Total Diario Estimado:** **1.016.667 COP por persona**
-**Consideraciones Finales:**
-*   **Actividades:**  Este cálculo no incluye el costo de actividades como tours de avistamiento de aves, entradas a parques nacionales, etc.  Estos costos pueden variar significativamente.  Es importante investigar y presupuestar estas actividades por separado.
-*   **Seguro de Viaje:**  Es fundamental contar con un seguro de viaje, lo cual agregaría un costo adicional.
-*   **Flexibilidad:**  Es importante tener flexibilidad en el presupuesto, ya que pueden surgir gastos inesperados.
-*   **Negociación:**  En algunos casos, es posible negociar precios, especialmente en alojamientos y tours locales.
+          <t>Con base en la información y resultados web, calcule el **costo total del viaje** en COP, desglosado por:
+- Transporte (tiquetes incluidos): total y por persona.
+- Alojamiento: total y por persona.
+- Alimentación: total y por persona.
+Para estimar el costo del viaje, necesito hacer algunas suposiciones y usar rangos de precios promedio, ya que la información proporcionada es limitada.  Es importante recordar que estos son solo estimados y los precios reales pueden variar significativamente dependiendo de las elecciones específicas (aerolínea, hotel, restaurantes, etc.).
+**Suposiciones:**
+*   **Tiquetes:** Asumo un precio promedio para un tiquete ida y vuelta Pereira - Roma.
+*   **Alojamiento:** Asumo un hotel de gama media (3 estrellas) o un Airbnb con buena ubicación.
+*   **Comida:** Asumo un presupuesto moderado para comidas, incluyendo restaurantes locales y algunas experiencias gastronómicas.
+*   **Transporte local:** Incluyo transporte público y algunos taxis/ubers.
+*   **Número de viajeros:** Asumo que viaja **1 persona**, ya que no se especifica. Si viajan más personas, el costo por persona de alojamiento podría disminuir.
+**Estimaciones:**
+**1. Tiquetes (Ida y Vuelta Pereira - Roma):**
+*   Rango estimado: COP 4.000.000 - COP 7.000.000 (Dependiendo de la temporada, aerolínea y anticipación de la compra).
+*   Promedio estimado: COP 5.500.000
+**2. Alojamiento (por noche):**
+*   Rango estimado: COP 300.000 - COP 600.000 (Hotel 3 estrellas o Airbnb bien ubicado).
+*   Promedio estimado: COP 450.000
+**3. Comida (por día):**
+*   Rango estimado: COP 150.000 - COP 300.000 (Incluyendo desayuno, almuerzo, cena y alguna experiencia gastronómica).
+*   Promedio estimado: COP 225.000
+**4. Transporte Local (por día):**
+*   Rango estimado: COP 30.000 - COP 60.000 (Transporte público, algunos taxis/ubers).
+*   Promedio estimado: COP 45.000
+**Cálculos:**
+*   **Costo total de alojamiento (4 noches):** 4 noches * COP 450.000/noche = COP 1.800.000
+*   **Costo total de comida (4 días):** 4 días * COP 225.000/día = COP 900.000
+*   **Costo total de transporte local (4 días):** 4 días * COP 45.000/día = COP 180.000
+**Resumen:**
+| Concepto        | Costo Total (COP) | Costo Diario (COP) | Costo Diario por Persona (COP) |
+|-----------------|--------------------|---------------------|---------------------------------|
+| Tiquetes        | 5.500.000          | 1.375.000 (prorrateado)  | 1.375.000                       |
+| Alojamiento     | 1.800.000          | 450.000             | 450.000                         |
+| Comida          | 900.000            | 225.000             | 225.000                         |
+| Transporte Local | 180.000            | 45.000              | 45.000                          |
+| **TOTAL**       | **8.380.000**      | **2.095.000**       | **2.095.000**                   |
 **Conclusión:**
-Con un presupuesto de 9 millones de COP para dos personas durante 6 días, el costo diario estimado de 1.016.667 COP por persona parece razonable, aunque es importante tener en cuenta las consideraciones finales y ajustar el presupuesto según las preferencias y actividades específicas del viaje.  Es crucial investigar los precios de los vuelos y alojamientos con anticipación para obtener una estimación más precisa.
+*   **Costo total estimado del viaje (4 días): COP 8.380.000**
+*   **Costo total diario estimado: COP 2.095.000**
+*   **Costo diario por persona estimado: COP 2.095.000**
+**Importante:**
+*   Estos son solo estimados.  Investigue a fondo los precios de vuelos y alojamiento para obtener una estimación más precisa.
+*   El costo de las actividades culturales (museos, tours, etc.) y otros gastos (souvenirs, etc.) no están incluidos en esta estimación.
+*   Los precios pueden variar significativamente dependiendo de la temporada alta/baja y la disponibilidad.
+*   Considere la tasa de cambio COP/EUR al momento de planificar su viaje.
+Para obtener una estimación más precisa, proporcione:
+*   Fechas específicas del viaje.
+*   Número de viajeros.
+*   Preferencias de alojamiento (hotel, Airbnb, presupuesto).
+*   Intereses específicos (actividades, restaurantes).
 Resultados de internet:
-Precios en San José Marzo 2025 precios en restaurantes, alimentos y ...: https://hikersbay.com/prices/costarica/p/san-jose?lang=es
-Costo de vida y precios en San José ... - TravelTables: https://es.traveltables.com/country/costa-rica/city/san-jose/cost-of-living/
-Precios de transportes y servicios en Costa Rica 2025: https://preciosmundi.com/costa-rica/precio-transporte-servicios
-Costo de vida en San Jose, Costa Rica, Costa Rica - Expatistan: https://www.expatistan.com/es/costo-de-vida/san-jose-costa-rica
-Costo de viaje: Guía económica de Costa Rica | El Blog del Viajero: https://elblogdelviajero.com/costo-de-viaje-costa-rica-2/
-Presente solo los valores aproximados por concepto.</t>
+Precios en Roma 2025 precios en restaurantes, alimentos y bebidas ...: https://hikersbay.com/prices/italy/rome?lang=es
+¿Cuánto dinero se necesita para visitar Roma? - HolboxPhotos: https://holboxphotos.com/roma/cuanto-dinero-se-necesita-para-visitar-roma/
+¿Cuánto dinero se gasta por día en Roma? | Felices Vacaciones: https://blog.felicesvacaciones.es/cuanto-dinero-se-gasta-por-dia-en-roma
+Precios en Roma, Transporte, Comida y bebidas, Alojamiento, Turismo: https://www.viajarroma.com/precios/
+¿Cuánto cuesta un viaje a Roma? Todos los días, 3 días y por semana ...: https://hikersbay.com/travel-cost/italy/rome?lang=es
+Solo muestre valores numéricos con etiquetas claras.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Aquí están los costos diarios estimados en COP por persona, basados en la información anterior:
-*   **Transporte:** 766.667 COP
-*   **Alojamiento:** 150.000 COP
-*   **Alimentación:** 100.000 COP</t>
+          <t>**Resumen de Costos Estimados del Viaje a Roma (COP):**
+*   **Tiquetes (Ida y Vuelta por persona):** 5.500.000
+*   **Alojamiento (Total, 4 noches):** 1.800.000
+*   **Alojamiento (Por persona, 4 noches):** 1.800.000
+*   **Alimentación (Total, 4 días):** 900.000
+*   **Alimentación (Por persona, 4 días):** 900.000
+*   **Transporte Local (Total, 4 días):** 180.000
+*   **Transporte Local (Por persona, 4 días):** 180.000
+*   **Costo Total Estimado del Viaje:** 8.380.000
+*   **Costo Diario Estimado por Persona:** 2.095.000</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-04-05 20:05:46</t>
+          <t>2025-04-06 15:31:08</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cálculo de Presupuesto</t>
+          <t>Consulta Tiquetes</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Con los siguientes costos estimados, calcule el total y compare con el presupuesto indicado por el usuario. Si excede, sugiera 1 o 2 formas de reducir gastos:
-Aquí están los costos diarios estimados en COP por persona, basados en la información anterior:
-*   **Transporte:** 766.667 COP
-*   **Alojamiento:** 150.000 COP
-*   **Alimentación:** 100.000 COP</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Okay, necesito más información para poder hacer el cálculo y la comparación. Necesito saber:
-1.  **Duración del viaje:** ¿Cuántos días dura el viaje?
-2.  **Número de personas:** ¿Cuántas personas están viajando?
-3.  **Presupuesto indicado por el usuario:** ¿Cuál es el presupuesto total que el usuario ha indicado para el viaje?
-Una vez que tenga esta información, puedo calcular el costo total estimado y compararlo con el presupuesto.  Luego, si el costo excede el presupuesto, puedo sugerir formas de reducir gastos.
-**Ejemplo:**
-Digamos que el viaje dura **5 días**, son **2 personas** viajando, y el presupuesto del usuario es de **3.000.000 COP**.
-**Cálculo:**
-*   **Transporte total:** 766.667 COP/persona/día * 2 personas * 5 días = 7.666.670 COP
-*   **Alojamiento total:** 150.000 COP/persona/día * 2 personas * 5 días = 1.500.000 COP
-*   **Alimentación total:** 100.000 COP/persona/día * 2 personas * 5 días = 1.000.000 COP
-*   **Costo total estimado:** 7.666.670 COP + 1.500.000 COP + 1.000.000 COP = 10.166.670 COP
-**Comparación:**
-El costo total estimado (10.166.670 COP) excede el presupuesto del usuario (3.000.000 COP) por 7.166.670 COP.
-**Sugerencias para reducir gastos (en este ejemplo):**
-1.  **Transporte:** El transporte es el gasto más grande.  Investigar opciones de transporte más económicas.  ¿Es posible usar transporte público en lugar de taxis o servicios de transporte privado?  ¿Se pueden encontrar vuelos o buses más baratos?  Considerar viajar en horarios menos demandados.
-2.  **Alojamiento:** Buscar opciones de alojamiento más económicas.  Considerar hostales, Airbnb (buscando opciones más económicas), o alojamientos fuera de las zonas más turísticas.
-**Por favor, proporciona la duración del viaje, el número de personas y el presupuesto del usuario para que pueda hacer un cálculo preciso y ofrecer sugerencias personalizadas.**</t>
-        </is>
-      </c>
+          <t>Precio promedio tiquetes pereira roma italia</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-04-05 20:05:53</t>
+          <t>2025-04-06 15:31:10</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Resultados Tiquetes</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Precio promedio tiquetes pereira roma italia</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Vuelos Baratos de Pereira a Roma - Despegar: https://www.despegar.com.co/vuelos/pei/rom/vuelos-a-roma-desde-pereira
+$2.169.116 | Vuelos baratos desde Pereira a Roma (PEI - ROM) - KAYAK: https://www.kayak.com.co/vuelos/Pereira-Matecana-PEI/Roma-ROM
+Vuelos baratos de Pereira, Colombia a Roma, Italia - Kiwi.com: https://www.kiwi.com/es/cheap-flights/pereira-colombia/rome-italy/
+$1.994.034 Reserva vuelos baratos de Pereira a Roma-Fiumicino (PEI ...: https://www.kayak.com.co/vuelos/Pereira-Matecana-PEI/Roma-Fiumicino-FCO
+Vuelos Pereira-Roma desde $ 4.869.072 - Viajala: https://viajala.com.co/vuelos-de-pereira-a-roma-PEI-ROM</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:31:14</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Cálculo de Presupuesto</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Tienes estos costos totales del viaje en COP:
+8380000
+Y esta información del usuario (incluye presupuesto):
+{'presupuesto': '5 millones'}
+1. Extrae el presupuesto del usuario.
+2. Compara el presupuesto con el **costo total**:
+   - Si el presupuesto ≥ costo total: confirma que cubre los gastos y muestra qué % representa cada concepto.
+   - Si el presupuesto &lt; costo total: indica que NO es suficiente y sugiere 2 ajustes al plan.
+No hagas desglose del presupuesto si no alcanza.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>```python
+costo_total = 8380000
+info_usuario = {'presupuesto': '5 millones'}
+# 1. Extraer el presupuesto del usuario
+presupuesto_str = info_usuario['presupuesto']
+# Eliminar " millones" y convertir a entero, multiplicando por 1 millón
+presupuesto = int(presupuesto_str.replace(' millones', '')) * 1000000
+# 2. Comparar el presupuesto con el costo total
+if presupuesto &gt;= costo_total:
+    print("¡Felicidades! Tu presupuesto cubre el costo total del viaje.")
+    # Calcular el porcentaje que representa el costo total del presupuesto
+    porcentaje_costo = (costo_total / presupuesto) * 100
+    print(f"El costo total del viaje representa el {porcentaje_costo:.2f}% de tu presupuesto.")
+else:
+    print("Lo sentimos, tu presupuesto NO es suficiente para cubrir el costo total del viaje.")
+    print("Te sugerimos los siguientes ajustes al plan:")
+    print("- **Reducir la duración del viaje:** Considera acortar el viaje en unos días para disminuir los gastos de alojamiento y actividades.")
+    print("- **Buscar opciones de alojamiento más económicas:** Explora hostales, apartamentos o alojamientos fuera de las zonas más turísticas.")
+```
+**Explicación del código:**
+1. **Extracción del presupuesto:**
+   - Se extrae el valor del presupuesto del diccionario `info_usuario`.
+   - Se utiliza `replace(' millones', '')` para eliminar la cadena " millones" del string.
+   - Se convierte el string resultante a un entero usando `int()`.
+   - Se multiplica por 1,000,000 para convertirlo a la cantidad numérica correcta (en COP).
+2. **Comparación y salida:**
+   - Se compara el `presupuesto` con el `costo_total`.
+   - **Si el presupuesto es suficiente:**
+     - Se imprime un mensaje de felicitación.
+     - Se calcula el porcentaje que representa el costo total del presupuesto.
+     - Se imprime el porcentaje formateado a dos decimales usando `:.2f`.
+   - **Si el presupuesto no es suficiente:**
+     - Se imprime un mensaje indicando que el presupuesto no es suficiente.
+     - Se sugieren dos ajustes al plan de viaje: reducir la duración y buscar alojamiento más económico.
+**Salida del código:**
+```
+Lo sentimos, tu presupuesto NO es suficiente para cubrir el costo total del viaje.
+Te sugerimos los siguientes ajustes al plan:
+- **Reducir la duración del viaje:** Considera acortar el viaje en unos días para disminuir los gastos de alojamiento y actividades.
+- **Buscar opciones de alojamiento más económicas:** Explora hostales, apartamentos o alojamientos fuera de las zonas más turísticas.
+```</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:31:26</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>Itinerario Final</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Con base en la siguiente información, genere un itinerario de viaje detallado pero conciso:
-0. Preferencias del usuario:
-```json
-{
-  "origen": "Pasto",
-  "destino": "Costa Rica",
-  "fecha": "Noviembre",
-  "duracion": "5-7 días",
-  "tipo_viaje": "Turismo ecológico",
-  "acompanantes": "Un amigo",
-  "presupuesto": "8-10 millones",
-  "expectativas": "Avistamiento de aves"
-}
-```
-1. Requisitos migratorios: Con base en la información proporcionada y los resultados web, los requisitos migratorios para colombianos que viajan a Costa Rica para turismo ecológico en noviembre son:
-*   **Visa:** Dependiendo de tu nacionalidad, es posible que necesites una visa. Consulta los enlaces proporcionados, especialmente el de la Embajada de Costa Rica en Colombia, para determinar si necesitas visa.
-*   **Pasaporte:** Pasaporte vigente con al menos seis meses de validez al momento del ingreso.
-*   **Tiquete de salida:** Billete de avión de salida de Costa Rica (ida y vuelta).
-*   **Prueba de solvencia económica:** Demostrar que se cuenta con los recursos económicos suficientes para cubrir los gastos durante la estadía.
-*   **Vacunas:** No se exigen vacunas obligatorias para ingresar a Costa Rica desde Colombia.
-*   **Otros documentos:** Es recomendable llevar una copia de la reserva del hotel o lugar de hospedaje, así como un itinerario del viaje.
-**Importante:**
-*   Verifica la información más actualizada en los sitios web oficiales de la Embajada de Costa Rica en Colombia y Visit Costa Rica, ya que los requisitos pueden cambiar.
-*   Asegúrate de cumplir con todos los requisitos para evitar problemas al ingresar al país.
-2. Información turística: Aquí está un resumen del clima, eventos y temporada turística en Costa Rica en Noviembre, basado en la información proporcionada y los resultados de búsqueda:
-*   **Clima:** Noviembre representa la transición de la temporada de lluvias a la seca.
-    *   **Pacífico:** Disminuyen las lluvias, con días soleados intercalados.
-    *   **Caribe:** Generalmente más lluvioso que el Pacífico.
-    *   En general, se puede esperar lluvia, pero no constante.
-*   **Temporada Turística:** Temporada baja/media.
-    *   Menos multitudes en comparación con la temporada alta (Diciembre-Abril).
-    *   Precios más bajos en alojamiento y tours.
-*   **Eventos/Actividades:**
-    *   Avistamiento de aves migratorias (oportunidad destacada).
-    *   Aunque no se mencionan eventos nacionales específicos, el clima en transición y la menor afluencia de turistas hacen de Noviembre un buen momento para explorar el país.
-3. Presupuesto y costos estimados: Okay, necesito más información para poder hacer el cálculo y la comparación. Necesito saber:
-1.  **Duración del viaje:** ¿Cuántos días dura el viaje?
-2.  **Número de personas:** ¿Cuántas personas están viajando?
-3.  **Presupuesto indicado por el usuario:** ¿Cuál es el presupuesto total que el usuario ha indicado para el viaje?
-Una vez que tenga esta información, puedo calcular el costo total estimado y compararlo con el presupuesto.  Luego, si el costo excede el presupuesto, puedo sugerir formas de reducir gastos.
-**Ejemplo:**
-Digamos que el viaje dura **5 días**, son **2 personas** viajando, y el presupuesto del usuario es de **3.000.000 COP**.
-**Cálculo:**
-*   **Transporte total:** 766.667 COP/persona/día * 2 personas * 5 días = 7.666.670 COP
-*   **Alojamiento total:** 150.000 COP/persona/día * 2 personas * 5 días = 1.500.000 COP
-*   **Alimentación total:** 100.000 COP/persona/día * 2 personas * 5 días = 1.000.000 COP
-*   **Costo total estimado:** 7.666.670 COP + 1.500.000 COP + 1.000.000 COP = 10.166.670 COP
-**Comparación:**
-El costo total estimado (10.166.670 COP) excede el presupuesto del usuario (3.000.000 COP) por 7.166.670 COP.
-**Sugerencias para reducir gastos (en este ejemplo):**
-1.  **Transporte:** El transporte es el gasto más grande.  Investigar opciones de transporte más económicas.  ¿Es posible usar transporte público en lugar de taxis o servicios de transporte privado?  ¿Se pueden encontrar vuelos o buses más baratos?  Considerar viajar en horarios menos demandados.
-2.  **Alojamiento:** Buscar opciones de alojamiento más económicas.  Considerar hostales, Airbnb (buscando opciones más económicas), o alojamientos fuera de las zonas más turísticas.
-**Por favor, proporciona la duración del viaje, el número de personas y el presupuesto del usuario para que pueda hacer un cálculo preciso y ofrecer sugerencias personalizadas.**
-Presente el resultado en las siguientes secciones:
-**I. Documentos y requisitos:**
-- Enumere los documentos necesarios para el ingreso y salida del país.
-- Indique si se necesita visa, vacunas, o formularios especiales.
-**II. Información general del destino:**
-- Clima estimado en las fechas del viaje.
-- Temporada (alta o baja).
-- Eventos especiales que coincidan con el viaje.
-**III. Presupuesto estimado:**
-- Desglose en COP por transporte, alojamiento y alimentación.
-- Nota si se ajusta al presupuesto definido o si se requieren cambios.
-**IV. Itinerario diario sugerido:**
-Presente de forma breve un plan por día. Para cada día, indique:
-- Actividades principales (máximo 3 por día).
-- Tipo de actividad (cultural, gastronómica, naturaleza, descanso, etc.).
-- Sugerencias de horario o ubicación si aplica.
-**V. Recomendaciones finales:**
-- Consejos adicionales según el perfil del viaje (por ejemplo, si es romántico, familiar, de aventura, etc.).
-- Recomendaciones sobre transporte local, seguridad o reservas anticipadas.
-El texto debe ser claro, útil y concreto. Use listas o viñetas cuando sea posible para facilitar la lectura.</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Aquí tienes un itinerario detallado y conciso para tu viaje de turismo ecológico a Costa Rica, basado en la información proporcionada y asumiendo una duración de **7 días**, **2 personas** viajando, y un presupuesto de **9.000.000 COP**.
-**I. Documentos y requisitos:**
-*   **Pasaporte:** Vigente con al menos seis meses de validez al momento del ingreso.
-*   **Tiquete de salida:** Billete de avión de salida de Costa Rica (ida y vuelta).
-*   **Prueba de solvencia económica:** Demostrar que se cuenta con los recursos económicos suficientes para cubrir los gastos durante la estadía (extractos bancarios, tarjetas de crédito).
-*   **Visa:** Verificar si se necesita visa según la nacionalidad. Consultar la Embajada de Costa Rica en Colombia.
-*   **Vacunas:** No se exigen vacunas obligatorias.
-*   **Otros documentos:** Copia de la reserva del hotel o lugar de hospedaje, itinerario del viaje.
-**II. Información general del destino:**
-*   **Clima estimado:** Transición de la temporada de lluvias a la seca. En el Pacífico, menos lluvias con días soleados. En el Caribe, más lluvioso. Esperar lluvia, pero no constante.
-*   **Temporada:** Baja/media. Menos multitudes y precios más bajos.
-*   **Eventos especiales:** Avistamiento de aves migratorias. No hay eventos nacionales específicos en noviembre, pero es un buen momento para explorar el país con menos turistas.
-**III. Presupuesto estimado:**
-Para un viaje de 7 días y 2 personas, con un presupuesto de 9.000.000 COP, se recomienda lo siguiente (aproximado y adaptable):
-*   **Transporte (vuelos y transporte interno):** 4.500.000 COP (2.250.000 COP por persona).  Buscar vuelos económicos y considerar transporte público o compartido dentro de Costa Rica.
-*   **Alojamiento:** 2.100.000 COP (150.000 COP por persona por noche).  Optar por alojamientos ecológicos más económicos como cabañas, hostales o Airbnb fuera de las zonas más turísticas.
-*   **Alimentación:** 1.400.000 COP (100.000 COP por persona por día).  Comer en sodas (restaurantes locales) y preparar algunas comidas para ahorrar.
-*   **Actividades y entradas:** 1.000.000 COP (500.000 COP por persona). Priorizar actividades gratuitas o de bajo costo como caminatas y visitar parques nacionales.
-**Nota:** Este presupuesto es ajustado.  Se recomienda buscar ofertas en vuelos y alojamiento, y ser flexible con las actividades.
-**IV. Itinerario diario sugerido:**
-*   **Día 1: Llegada a San José y traslado a La Fortuna (Arenal).**
-    *   Actividad principal: Traslado desde el aeropuerto Juan Santamaría (SJO) a La Fortuna.
-    *   Tipo de actividad: Traslado, naturaleza.
-    *   Sugerencia: Reservar un transporte compartido o bus para reducir costos.
-*   **Día 2: Volcán Arenal y aguas termales.**
-    *   Actividades principales: Caminata por senderos alrededor del Volcán Arenal, visita a aguas termales (Baldi, Tabacon, Ecotermales Fortuna - este último más económico).
-    *   Tipo de actividad: Naturaleza, relajación.
-    *   Sugerencia: Elegir aguas termales más económicas y reservar con anticipación.
-*   **Día 3: La Fortuna - Monteverde.**
-    *   Actividades principales: Traslado de La Fortuna a Monteverde (Jeep-Boat-Jeep es una opción escénica), caminata por la tarde en la Reserva Biológica Bosque Nuboso Monteverde.
-    *   Tipo de actividad: Traslado, naturaleza.
-    *   Sugerencia: Reservar el traslado Jeep-Boat-Jeep con anticipación.
-*   **Día 4: Monteverde - Canopy y puentes colgantes.**
-    *   Actividades principales: Canopy (tirolesa) en el bosque nuboso, caminata por los puentes colgantes.
-    *   Tipo de actividad: Aventura, naturaleza.
-    *   Sugerencia: Comparar precios de diferentes operadores de canopy.
-*   **Día 5: Monteverde - Manuel Antonio.**
-    *   Actividades principales: Traslado de Monteverde a Manuel Antonio.
-    *   Tipo de actividad: Traslado.
-    *   Sugerencia: Considerar un bus directo para ahorrar.
-*   **Día 6: Parque Nacional Manuel Antonio.**
-    *   Actividades principales: Visita al Parque Nacional Manuel Antonio (playas, senderos, avistamiento de fauna).
-    *   Tipo de actividad: Naturaleza, playa.
-    *   Sugerencia: Llegar temprano al parque para evitar multitudes.
-*   **Día 7: Regreso a San José y salida.**
-    *   Actividades principales: Traslado de Manuel Antonio a San José, vuelo de regreso a Pasto.
-    *   Tipo de actividad: Traslado.
-    *   Sugerencia: Reservar el transporte con anticipación.
-**V. Recomendaciones finales:**
-*   **Turismo ecológico:** Respetar la flora y fauna local. No alimentar a los animales. Utilizar protector solar biodegradable.
-*   **Transporte local:** El transporte público en Costa Rica es relativamente económico, pero puede ser lento. Considerar buses o transporte compartido para traslados largos.
-*   **Seguridad:** Costa Rica es generalmente segura, pero tomar precauciones básicas como no dejar objetos de valor a la vista y estar atento a los alrededores.
-*   **Reservas anticipadas:** Reservar alojamiento y tours con anticipación, especialmente si viajan en temporada alta (aunque noviembre es temporada baja/media).
-*   **Avistamiento de aves:** Llevar binoculares y una guía de aves de Costa Rica. Contratar un guía local para aumentar las posibilidades de avistamiento.
-*   **Flexibilidad:** Ser flexible con el itinerario y estar preparado para cambios debido al clima.
-*   **Idioma:** Aunque el español es el idioma oficial, el inglés es ampliamente hablado en las zonas turísticas.
-Este itinerario es una sugerencia y puede ser adaptado a tus intereses y presupuesto. ¡Disfruta tu viaje a Costa Rica!</t>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>¡Prepárese para vivir la experiencia de su vida con DaviTravel! A continuación encontrará un itinerario ideal para el viaje de sus sueños:
+0. **Preferencias de viaje:**
+{'origen': 'pereira', 'destino': 'roma, italia', 'fecha': 'verano europa', 'duracion': '4', 'tipo_viaje': 'cultural y gastronomico', 'acompanantes': 'solo', 'presupuesto': '5 millones', 'expectativas': 'comer la mejor pasta'}
+1. **Requisitos migratorios:**
+Para viajar de Pereira a Roma, Italia, los requisitos migratorios generales son:
+*   **Visa:** No se requiere visa para estancias turísticas cortas (hasta 90 días).
+*   **Pasaporte:** Pasaporte válido con una vigencia de al menos 3 meses después de la fecha prevista de salida de Italia/Espacio Schengen.
+*   **Tiquete de Regreso:** Billete de avión de ida y vuelta.
+*   **Justificación del Viaje:** Documentación que justifique el propósito del viaje (ej: reservas de hotel, itinerario turístico).
+*   **Solvencia Económica:** Demostrar que se cuenta con los recursos económicos suficientes.
+*   **Seguro de Viaje:** Es obligatorio contar con un seguro de viaje con cobertura médica internacional con una cobertura mínima de 30.000 euros.
+*   **Vacunas:** No hay vacunas obligatorias.
+*   **Formulario de localización de pasajeros (PLF):** Es posible que se requiera completar un formulario de localización de pasajeros (PLF).
+**Recomendaciones Adicionales:**
+*   **Consulta las fuentes oficiales:** Verifica la información directamente en las páginas web de la Embajada de Italia en Colombia y la Cancillería de Colombia para obtener la información más actualizada y precisa.
+*   **Considera posibles cambios:** Los requisitos pueden cambiar, especialmente en lo relacionado con la pandemia. Mantente informado cerca de la fecha de tu viaje.
+2. **Información turística:**
+Clima: Caluroso y seco.
+Temporada Turística: Alta.
+Eventos: Festivales al aire libre, Conciertos, Eventos culturales, Celebraciones religiosas.
+3. **Presupuesto y costos estimados:**
+Lo sentimos, tu presupuesto NO es suficiente para cubrir el costo total del viaje.
+Te sugerimos los siguientes ajustes al plan:
+- **Reducir la duración del viaje:** Considera acortar el viaje en unos días para disminuir los gastos de alojamiento y actividades.
+- **Buscar opciones de alojamiento más económicas:** Explora hostales, apartamentos o alojamientos fuera de las zonas más turísticas.
+Organice el plan en estas secciones:
+I. **Documentos y requisitos**
+- Documentos imprescindibles para ingreso y salida.
+- Visa, vacunas u otros permisos necesarios.
+II. **Resumen del destino**
+- Clima en las fechas seleccionadas.
+- Temporada (alta o baja) y eventos especiales.
+III. **Desglose de presupuesto**
+- Transporte, alojamiento y alimentación en COP.
+- Indique si el plan se ajusta al presupuesto o sugiera ajustes.
+IV. **Itinerario diario**
+Para cada día, proponga:
+- Hasta 3 actividades destacadas.
+- Tipo de experiencia (cultural, gastronómica, aventura, descanso).
+- Horarios recomendados y ubicaciones clave.
+V. **Toques finales**
+- Consejos exclusivos según su perfil de viaje.
+- Recomendaciones de reservas anticipadas y transporte local.
+Haga que cada momento sea inolvidable y despierte la emoción de su próxima aventura.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>¡Absolutamente! Aquí tienes un itinerario diseñado para tu viaje a Roma, adaptado a tus preferencias y presupuesto, con los ajustes necesarios:
+**I. Documentos y Requisitos**
+*   **Documentos Imprescindibles:**
+    *   Pasaporte: Con vigencia de al menos 3 meses después de la fecha de regreso prevista (¡Verifica la fecha de expiración!).
+    *   Tiquete de avión de ida y vuelta.
+    *   Comprobante de alojamiento (reservas de hotel/hostal).
+    *   Seguro de viaje: Con cobertura médica internacional de al menos 30,000 euros.
+*   **Visa:** No requerida para estancias turísticas de hasta 90 días.
+*   **Vacunas:** No obligatorias.
+*   **Formulario de Localización de Pasajeros (PLF):** Verifica si es necesario completarlo cerca de la fecha de viaje.
+**II. Resumen del Destino**
+*   **Clima en Verano:** Caluroso y seco, con temperaturas que pueden superar los 30°C. Lleva ropa ligera, protector solar y un sombrero.
+*   **Temporada:** Alta (junio-agosto). Roma estará llena de turistas, así que prepárate para las multitudes y reserva todo con anticipación.
+*   **Eventos:** Festivales al aire libre, conciertos, eventos culturales, celebraciones religiosas (consulta la programación local antes de viajar).
+**III. Desglose de Presupuesto (Ajustado)**
+Dado que tu presupuesto de 5 millones de COP es limitado para un viaje de 4 días a Roma en temporada alta, he ajustado el itinerario para que sea más económico.
+*   **Transporte (Ida y Vuelta):** 2,500,000 COP (aproximado, puede variar según la aerolínea y la anticipación de la compra).
+*   **Alojamiento (Hostal/Airbnb):** 800,000 COP (4 noches x 200,000 COP por noche).
+*   **Alimentación:** 1,000,000 COP (250,000 COP por día). Prioriza trattorias locales y mercados para ahorrar.
+*   **Actividades/Entradas:** 500,000 COP (considerando algunas atracciones gratuitas y otras de bajo costo).
+*   **Transporte Local:** 200,000 COP (metro, autobús).
+**Total Estimado:** 5,000,000 COP
+**Ajustes Clave:**
+*   **Alojamiento:** Opta por un hostal o un Airbnb fuera del centro histórico para ahorrar en alojamiento.
+*   **Comida:** Evita los restaurantes turísticos caros. Busca trattorias locales y mercados para disfrutar de la auténtica cocina romana a precios más asequibles.
+*   **Actividades:** Aprovecha las atracciones gratuitas (iglesias, plazas, parques) y considera comprar un Roma Pass para obtener descuentos en transporte y museos.
+**IV. Itinerario Diario**
+**Día 1: Llegada y Roma Antigua**
+*   **Mañana (9:00 AM):** Llegada al aeropuerto de Fiumicino (FCO). Toma el tren Leonardo Express hasta la estación Termini (14 euros).
+    *   *Experiencia:* Traslado y primer contacto con la ciudad.
+*   **Tarde (12:00 PM):** Check-in en el hostal/Airbnb.
+    *   *Experiencia:* Acomodación.
+*   **Tarde (2:00 PM):** Coliseo y Foro Romano (compra las entradas en línea con anticipación para evitar filas).
+    *   *Experiencia:* Cultural e histórica.
+    *   *Ubicación:* Coliseo, Foro Romano.
+*   **Noche (7:00 PM):** Cena en una trattoria local en el barrio Monti.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Trattoria Ai Tre Scalini.
+**Día 2: Vaticano y Centro Histórico**
+*   **Mañana (9:00 AM):** Ciudad del Vaticano: Basílica de San Pedro y Museos Vaticanos (reserva las entradas en línea para evitar filas).
+    *   *Experiencia:* Cultural y religiosa.
+    *   *Ubicación:* Ciudad del Vaticano.
+*   **Tarde (2:00 PM):** Castillo de Sant'Angelo.
+    *   *Experiencia:* Cultural e histórica.
+    *   *Ubicación:* Castillo de Sant'Angelo.
+*   **Tarde (5:00 PM):** Paseo por el centro histórico: Piazza Navona, Panteón, Fontana di Trevi.
+    *   *Experiencia:* Cultural y visual.
+    *   *Ubicación:* Centro histórico.
+*   **Noche (8:00 PM):** Cena en el barrio Trastevere.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Trastevere.
+**Día 3: Arte y Jardines**
+*   **Mañana (10:00 AM):** Galería Borghese y Jardines de Villa Borghese (reserva con anticipación).
+    *   *Experiencia:* Cultural y natural.
+    *   *Ubicación:* Villa Borghese.
+*   **Tarde (2:00 PM):** Piazza del Popolo y Via del Corso.
+    *   *Experiencia:* Visual y comercial.
+    *   *Ubicación:* Piazza del Popolo, Via del Corso.
+*   **Tarde (5:00 PM):** Escalinata de la Plaza de España.
+    *   *Experiencia:* Visual.
+    *   *Ubicación:* Plaza de España.
+*   **Noche (7:00 PM):** Cena en el barrio Testaccio.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Testaccio.
+**Día 4: Despedida y Regreso**
+*   **Mañana (10:00 AM):** Mercado de Campo de' Fiori.
+    *   *Experiencia:* Gastronómica y cultural.
+    *   *Ubicación:* Campo de' Fiori.
+*   **Tarde (1:00 PM):** Almuerzo de despedida: ¡Disfruta de tu última pasta en Roma!
+    *   *Experiencia:* Gastronómica.
+*   **Tarde (4:00 PM):** Traslado al aeropuerto de Fiumicino (FCO).
+    *   *Experiencia:* Traslado.
+*   **Noche (7:00 PM):** Vuelo de regreso a Pereira.
+**V. Toques Finales**
+*   **Consejos Exclusivos:**
+    *   **Pasta:** Prueba la carbonara, cacio e pepe y amatriciana.
+    *   **Gelato:** No te pierdas las heladerías artesanales.
+    *   **Café:** Disfruta de un espresso en un bar local.
+*   **Reservas Anticipadas:**
+    *   Vuelos y alojamiento.
+    *   Coliseo, Museos Vaticanos, Galería Borghese.
+*   **Transporte Local:**
+    *   Metro: Eficiente para moverse por la ciudad.
+    *   Autobús: Útil para llegar a lugares fuera del centro.
+    *   Roma Pass: Considera comprarlo si planeas visitar muchos museos.
+¡Espero que este itinerario te ayude a planificar un viaje inolvidable a Roma!</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:31:44</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Integración Alianzas Davivienda</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>System: Usted es DaviTravel: siempre responde en español, en tercera persona, con entusiasmo y cercanía al usuario.
+Human: Toma este itinerario:
+¡Absolutamente! Aquí tienes un itinerario diseñado para tu viaje a Roma, adaptado a tus preferencias y presupuesto, con los ajustes necesarios:
+**I. Documentos y Requisitos**
+*   **Documentos Imprescindibles:**
+    *   Pasaporte: Con vigencia de al menos 3 meses después de la fecha de regreso prevista (¡Verifica la fecha de expiración!).
+    *   Tiquete de avión de ida y vuelta.
+    *   Comprobante de alojamiento (reservas de hotel/hostal).
+    *   Seguro de viaje: Con cobertura médica internacional de al menos 30,000 euros.
+*   **Visa:** No requerida para estancias turísticas de hasta 90 días.
+*   **Vacunas:** No obligatorias.
+*   **Formulario de Localización de Pasajeros (PLF):** Verifica si es necesario completarlo cerca de la fecha de viaje.
+**II. Resumen del Destino**
+*   **Clima en Verano:** Caluroso y seco, con temperaturas que pueden superar los 30°C. Lleva ropa ligera, protector solar y un sombrero.
+*   **Temporada:** Alta (junio-agosto). Roma estará llena de turistas, así que prepárate para las multitudes y reserva todo con anticipación.
+*   **Eventos:** Festivales al aire libre, conciertos, eventos culturales, celebraciones religiosas (consulta la programación local antes de viajar).
+**III. Desglose de Presupuesto (Ajustado)**
+Dado que tu presupuesto de 5 millones de COP es limitado para un viaje de 4 días a Roma en temporada alta, he ajustado el itinerario para que sea más económico.
+*   **Transporte (Ida y Vuelta):** 2,500,000 COP (aproximado, puede variar según la aerolínea y la anticipación de la compra).
+*   **Alojamiento (Hostal/Airbnb):** 800,000 COP (4 noches x 200,000 COP por noche).
+*   **Alimentación:** 1,000,000 COP (250,000 COP por día). Prioriza trattorias locales y mercados para ahorrar.
+*   **Actividades/Entradas:** 500,000 COP (considerando algunas atracciones gratuitas y otras de bajo costo).
+*   **Transporte Local:** 200,000 COP (metro, autobús).
+**Total Estimado:** 5,000,000 COP
+**Ajustes Clave:**
+*   **Alojamiento:** Opta por un hostal o un Airbnb fuera del centro histórico para ahorrar en alojamiento.
+*   **Comida:** Evita los restaurantes turísticos caros. Busca trattorias locales y mercados para disfrutar de la auténtica cocina romana a precios más asequibles.
+*   **Actividades:** Aprovecha las atracciones gratuitas (iglesias, plazas, parques) y considera comprar un Roma Pass para obtener descuentos en transporte y museos.
+**IV. Itinerario Diario**
+**Día 1: Llegada y Roma Antigua**
+*   **Mañana (9:00 AM):** Llegada al aeropuerto de Fiumicino (FCO). Toma el tren Leonardo Express hasta la estación Termini (14 euros).
+    *   *Experiencia:* Traslado y primer contacto con la ciudad.
+*   **Tarde (12:00 PM):** Check-in en el hostal/Airbnb.
+    *   *Experiencia:* Acomodación.
+*   **Tarde (2:00 PM):** Coliseo y Foro Romano (compra las entradas en línea con anticipación para evitar filas).
+    *   *Experiencia:* Cultural e histórica.
+    *   *Ubicación:* Coliseo, Foro Romano.
+*   **Noche (7:00 PM):** Cena en una trattoria local en el barrio Monti.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Trattoria Ai Tre Scalini.
+**Día 2: Vaticano y Centro Histórico**
+*   **Mañana (9:00 AM):** Ciudad del Vaticano: Basílica de San Pedro y Museos Vaticanos (reserva las entradas en línea para evitar filas).
+    *   *Experiencia:* Cultural y religiosa.
+    *   *Ubicación:* Ciudad del Vaticano.
+*   **Tarde (2:00 PM):** Castillo de Sant'Angelo.
+    *   *Experiencia:* Cultural e histórica.
+    *   *Ubicación:* Castillo de Sant'Angelo.
+*   **Tarde (5:00 PM):** Paseo por el centro histórico: Piazza Navona, Panteón, Fontana di Trevi.
+    *   *Experiencia:* Cultural y visual.
+    *   *Ubicación:* Centro histórico.
+*   **Noche (8:00 PM):** Cena en el barrio Trastevere.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Trastevere.
+**Día 3: Arte y Jardines**
+*   **Mañana (10:00 AM):** Galería Borghese y Jardines de Villa Borghese (reserva con anticipación).
+    *   *Experiencia:* Cultural y natural.
+    *   *Ubicación:* Villa Borghese.
+*   **Tarde (2:00 PM):** Piazza del Popolo y Via del Corso.
+    *   *Experiencia:* Visual y comercial.
+    *   *Ubicación:* Piazza del Popolo, Via del Corso.
+*   **Tarde (5:00 PM):** Escalinata de la Plaza de España.
+    *   *Experiencia:* Visual.
+    *   *Ubicación:* Plaza de España.
+*   **Noche (7:00 PM):** Cena en el barrio Testaccio.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Testaccio.
+**Día 4: Despedida y Regreso**
+*   **Mañana (10:00 AM):** Mercado de Campo de' Fiori.
+    *   *Experiencia:* Gastronómica y cultural.
+    *   *Ubicación:* Campo de' Fiori.
+*   **Tarde (1:00 PM):** Almuerzo de despedida: ¡Disfruta de tu última pasta en Roma!
+    *   *Experiencia:* Gastronómica.
+*   **Tarde (4:00 PM):** Traslado al aeropuerto de Fiumicino (FCO).
+    *   *Experiencia:* Traslado.
+*   **Noche (7:00 PM):** Vuelo de regreso a Pereira.
+**V. Toques Finales**
+*   **Consejos Exclusivos:**
+    *   **Pasta:** Prueba la carbonara, cacio e pepe y amatriciana.
+    *   **Gelato:** No te pierdas las heladerías artesanales.
+    *   **Café:** Disfruta de un espresso en un bar local.
+*   **Reservas Anticipadas:**
+    *   Vuelos y alojamiento.
+    *   Coliseo, Museos Vaticanos, Galería Borghese.
+*   **Transporte Local:**
+    *   Metro: Eficiente para moverse por la ciudad.
+    *   Autobús: Útil para llegar a lugares fuera del centro.
+    *   Roma Pass: Considera comprarlo si planeas visitar muchos museos.
+¡Espero que este itinerario te ayude a planificar un viaje inolvidable a Roma!
+Y estas alianzas activas de Davivienda en hotelería y turismo:
+- **TÃ­tulo de producto**: SubtÃ­tulo de producto. Beneficio: Millas Acumule. Aplica para: . [INSCRÃBASE AQUÃ]({{ URL_FRONT }}producto/{{ product.seo_url }})
+Devuelve exactamente el mismo itinerario, pero **inserta** en cada sección recomendaciones concretas de productos Davivienda (tarjetas, 0% interés, descuentos) para que el usuario aproveche al máximo las alianzas: desde la compra de tiquetes, reservas de alojamiento, actividades y compras locales. Mantén la estructura original y agrega en cada punto la sugerencia correspondiente.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>¡Claro que sí! DaviTravel ha revisado el itinerario y lo ha enriquecido con recomendaciones de productos Davivienda para que el viajero aproveche al máximo sus alianzas y beneficios. ¡Prepárense para una experiencia romana aún más completa!
+**I. Documentos y Requisitos**
+*   **Documentos Imprescindibles:**
+    *   Pasaporte: Con vigencia de al menos 3 meses después de la fecha de regreso prevista (¡Verifica la fecha de expiración!).
+    *   Tiquete de avión de ida y vuelta.
+    *   Comprobante de alojamiento (reservas de hotel/hostal).
+    *   Seguro de viaje: Con cobertura médica internacional de al menos 30,000 euros.
+*   **Visa:** No requerida para estancias turísticas de hasta 90 días.
+*   **Vacunas:** No obligatorias.
+*   **Formulario de Localización de Pasajeros (PLF):** Verifica si es necesario completarlo cerca de la fecha de viaje.
+    **DaviTravel Recomienda:** Utiliza tu Tarjeta de Crédito Davivienda para comprar los tiquetes aéreos y acumula millas para tu próximo viaje. ¡Además, muchos seguros de viaje ofrecen descuentos al pagar con tarjetas Davivienda!
+**II. Resumen del Destino**
+*   **Clima en Verano:** Caluroso y seco, con temperaturas que pueden superar los 30°C. Lleva ropa ligera, protector solar y un sombrero.
+*   **Temporada:** Alta (junio-agosto). Roma estará llena de turistas, así que prepárate para las multitudes y reserva todo con anticipación.
+*   **Eventos:** Festivales al aire libre, conciertos, eventos culturales, celebraciones religiosas (consulta la programación local antes de viajar).
+    **DaviTravel Recomienda:** Planifica tus compras de verano con anticipación y aprovecha las opciones de 0% de interés que ofrece Davivienda en comercios aliados. ¡Así podrás disfrutar del viaje sin preocuparte por el pago inmediato!
+**III. Desglose de Presupuesto (Ajustado)**
+Dado que tu presupuesto de 5 millones de COP es limitado para un viaje de 4 días a Roma en temporada alta, he ajustado el itinerario para que sea más económico.
+*   **Transporte (Ida y Vuelta):** 2,500,000 COP (aproximado, puede variar según la aerolínea y la anticipación de la compra).
+*   **Alojamiento (Hostal/Airbnb):** 800,000 COP (4 noches x 200,000 COP por noche).
+*   **Alimentación:** 1,000,000 COP (250,000 COP por día). Prioriza trattorias locales y mercados para ahorrar.
+*   **Actividades/Entradas:** 500,000 COP (considerando algunas atracciones gratuitas y otras de bajo costo).
+*   **Transporte Local:** 200,000 COP (metro, autobús).
+**Total Estimado:** 5,000,000 COP
+**Ajustes Clave:**
+*   **Alojamiento:** Opta por un hostal o un Airbnb fuera del centro histórico para ahorrar en alojamiento.
+*   **Comida:** Evita los restaurantes turísticos caros. Busca trattorias locales y mercados para disfrutar de la auténtica cocina romana a precios más asequibles.
+*   **Actividades:** Aprovecha las atracciones gratuitas (iglesias, plazas, parques) y considera comprar un Roma Pass para obtener descuentos en transporte y museos.
+    **DaviTravel Recomienda:** Busca alojamientos y actividades que tengan alianzas con Davivienda para obtener descuentos especiales. ¡Revisa la página web de Davivienda para conocer los beneficios vigentes!
+**IV. Itinerario Diario**
+**Día 1: Llegada y Roma Antigua**
+*   **Mañana (9:00 AM):** Llegada al aeropuerto de Fiumicino (FCO). Toma el tren Leonardo Express hasta la estación Termini (14 euros).
+    *   *Experiencia:* Traslado y primer contacto con la ciudad.
+*   **Tarde (12:00 PM):** Check-in en el hostal/Airbnb.
+    *   *Experiencia:* Acomodación.
+*   **Tarde (2:00 PM):** Coliseo y Foro Romano (compra las entradas en línea con anticipación para evitar filas).
+    *   *Experiencia:* Cultural e histórica.
+    *   *Ubicación:* Coliseo, Foro Romano.
+*   **Noche (7:00 PM):** Cena en una trattoria local en el barrio Monti.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Trattoria Ai Tre Scalini.
+    **DaviTravel Recomienda:** Utiliza tu Tarjeta Débito Davivienda para retirar euros en cajeros automáticos en Roma. ¡Así tendrás efectivo para gastos menores y evitarás comisiones altas por cambio de divisas!
+**Día 2: Vaticano y Centro Histórico**
+*   **Mañana (9:00 AM):** Ciudad del Vaticano: Basílica de San Pedro y Museos Vaticanos (reserva las entradas en línea para evitar filas).
+    *   *Experiencia:* Cultural y religiosa.
+    *   *Ubicación:* Ciudad del Vaticano.
+*   **Tarde (2:00 PM):** Castillo de Sant'Angelo.
+    *   *Experiencia:* Cultural e histórica.
+    *   *Ubicación:* Castillo de Sant'Angelo.
+*   **Tarde (5:00 PM):** Paseo por el centro histórico: Piazza Navona, Panteón, Fontana di Trevi.
+    *   *Experiencia:* Cultural y visual.
+    *   *Ubicación:* Centro histórico.
+*   **Noche (8:00 PM):** Cena en el barrio Trastevere.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Trastevere.
+    **DaviTravel Recomienda:** Si encuentras algún comercio en el Vaticano o en el centro histórico que acepte tarjetas, utiliza tu Tarjeta de Crédito Davivienda para acumular millas o puntos. ¡Cada compra cuenta!
+**Día 3: Arte y Jardines**
+*   **Mañana (10:00 AM):** Galería Borghese y Jardines de Villa Borghese (reserva con anticipación).
+    *   *Experiencia:* Cultural y natural.
+    *   *Ubicación:* Villa Borghese.
+*   **Tarde (2:00 PM):** Piazza del Popolo y Via del Corso.
+    *   *Experiencia:* Visual y comercial.
+    *   *Ubicación:* Piazza del Popolo, Via del Corso.
+*   **Tarde (5:00 PM):** Escalinata de la Plaza de España.
+    *   *Experiencia:* Visual.
+    *   *Ubicación:* Plaza de España.
+*   **Noche (7:00 PM):** Cena en el barrio Testaccio.
+    *   *Experiencia:* Gastronómica.
+    *   *Ubicación:* Testaccio.
+    **DaviTravel Recomienda:** ¡No olvides revisar si la Galería Borghese o algún comercio en Via del Corso tiene alianzas con Davivienda! Podrías obtener descuentos o beneficios adicionales al pagar con tus tarjetas.
+**Día 4: Despedida y Regreso**
+*   **Mañana (10:00 AM):** Mercado de Campo de' Fiori.
+    *   *Experiencia:* Gastronómica y cultural.
+    *   *Ubicación:* Campo de' Fiori.
+*   **Tarde (1:00 PM):** Almuerzo de despedida: ¡Disfruta de tu última pasta en Roma!
+    *   *Experiencia:* Gastronómica.
+*   **Tarde (4:00 PM):** Traslado al aeropuerto de Fiumicino (FCO).
+    *   *Experiencia:* Traslado.
+*   **Noche (7:00 PM):** Vuelo de regreso a Pereira.
+    **DaviTravel Recomienda:** Antes de regresar, revisa si tienes alguna compra pendiente y aprovecha los últimos momentos para utilizar tus tarjetas Davivienda y acumular millas o puntos. ¡Cada oportunidad cuenta!
+**V. Toques Finales**
+*   **Consejos Exclusivos:**
+    *   **Pasta:** Prueba la carbonara, cacio e pepe y amatriciana.
+    *   **Gelato:** No te pierdas las heladerías artesanales.
+    *   **Café:** Disfruta de un espresso en un bar local.
+*   **Reservas Anticipadas:**
+    *   Vuelos y alojamiento.
+    *   Coliseo, Museos Vaticanos, Galería Borghese.
+*   **Transporte Local:**
+    *   Metro: Eficiente para moverse por la ciudad.
+    *   Autobús: Útil para llegar a lugares fuera del centro.
+    *   Roma Pass: Considera comprarlo si planeas visitar muchos museos.
+    **DaviTravel Recomienda:** Antes de viajar, activa las notificaciones de tu aplicación Davivienda para estar al tanto de tus transacciones y mantener el control de tus gastos. ¡Así podrás disfrutar de tu viaje con tranquilidad!
+¡DaviTravel espera que este itinerario mejorado te ayude a planificar un viaje inolvidable a Roma, aprovechando al máximo los beneficios que Davivienda tiene para ti! ¡Buen viaje!</t>
         </is>
       </c>
     </row>

</xml_diff>